<commit_message>
Add Project File (.docx)
</commit_message>
<xml_diff>
--- a/docs/Taches a faire.xlsx
+++ b/docs/Taches a faire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\Eclipse Workspace\ecole\android\budget-monitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\Eclipse Workspace\ecole\android\budget-monitor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>A faire</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>A faire ensemble auourd'hui (vendredi)</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>Vicky</t>
+  </si>
+  <si>
+    <t>Nico</t>
   </si>
 </sst>
 </file>
@@ -377,7 +389,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,16 +409,25 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -425,10 +446,16 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated "Tache a faire" file
</commit_message>
<xml_diff>
--- a/docs/Taches a faire.xlsx
+++ b/docs/Taches a faire.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>A faire</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Qui ?</t>
   </si>
   <si>
-    <t>A faire ensemble auourd'hui (vendredi)</t>
-  </si>
-  <si>
     <t>Alex</t>
   </si>
   <si>
@@ -66,14 +63,45 @@
   </si>
   <si>
     <t>Nico</t>
+  </si>
+  <si>
+    <t>Etat avancement</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>A compléter si vous voyez d'autres choses a faire</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Ajoutez des actions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,11 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,79 +416,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>